<commit_message>
Added an install script
</commit_message>
<xml_diff>
--- a/outputs/dados.xlsx
+++ b/outputs/dados.xlsx
@@ -449,7 +449,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:31</t>
+          <t>02/03/2024 02:51:31</t>
         </is>
       </c>
       <c r="B2">
@@ -468,7 +468,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:41</t>
+          <t>02/03/2024 02:51:41</t>
         </is>
       </c>
       <c r="B3">
@@ -487,7 +487,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:51</t>
+          <t>02/03/2024 02:51:51</t>
         </is>
       </c>
       <c r="B4">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:01</t>
+          <t>02/03/2024 02:52:01</t>
         </is>
       </c>
       <c r="B5">
@@ -525,7 +525,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:11</t>
+          <t>02/03/2024 02:52:11</t>
         </is>
       </c>
       <c r="B6">
@@ -544,7 +544,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:21</t>
+          <t>02/03/2024 02:52:21</t>
         </is>
       </c>
       <c r="B7">
@@ -563,7 +563,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:31</t>
+          <t>02/03/2024 02:52:31</t>
         </is>
       </c>
       <c r="B8">
@@ -582,7 +582,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:41</t>
+          <t>02/03/2024 02:52:41</t>
         </is>
       </c>
       <c r="B9">
@@ -601,7 +601,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:51</t>
+          <t>02/03/2024 02:52:51</t>
         </is>
       </c>
       <c r="B10">
@@ -620,7 +620,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:01</t>
+          <t>02/03/2024 02:53:01</t>
         </is>
       </c>
       <c r="B11">
@@ -639,7 +639,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:11</t>
+          <t>02/03/2024 02:53:11</t>
         </is>
       </c>
       <c r="B12">
@@ -658,7 +658,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:21</t>
+          <t>02/03/2024 02:53:21</t>
         </is>
       </c>
       <c r="B13">
@@ -677,7 +677,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:31</t>
+          <t>02/03/2024 02:53:31</t>
         </is>
       </c>
       <c r="B14">
@@ -696,7 +696,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:41</t>
+          <t>02/03/2024 02:53:41</t>
         </is>
       </c>
       <c r="B15">
@@ -715,7 +715,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:51</t>
+          <t>02/03/2024 02:53:51</t>
         </is>
       </c>
       <c r="B16">
@@ -734,7 +734,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:01</t>
+          <t>02/03/2024 02:54:01</t>
         </is>
       </c>
       <c r="B17">
@@ -753,7 +753,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:11</t>
+          <t>02/03/2024 02:54:11</t>
         </is>
       </c>
       <c r="B18">
@@ -772,7 +772,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:21</t>
+          <t>02/03/2024 02:54:21</t>
         </is>
       </c>
       <c r="B19">
@@ -791,7 +791,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:31</t>
+          <t>02/03/2024 02:54:31</t>
         </is>
       </c>
       <c r="B20">
@@ -810,7 +810,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:41</t>
+          <t>02/03/2024 02:54:41</t>
         </is>
       </c>
       <c r="B21">
@@ -829,7 +829,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:51</t>
+          <t>02/03/2024 02:54:51</t>
         </is>
       </c>
       <c r="B22">
@@ -848,7 +848,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:01</t>
+          <t>02/03/2024 02:55:01</t>
         </is>
       </c>
       <c r="B23">
@@ -867,7 +867,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:11</t>
+          <t>02/03/2024 02:55:11</t>
         </is>
       </c>
       <c r="B24">
@@ -886,7 +886,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:21</t>
+          <t>02/03/2024 02:55:21</t>
         </is>
       </c>
       <c r="B25">
@@ -905,7 +905,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:31</t>
+          <t>02/03/2024 02:55:31</t>
         </is>
       </c>
       <c r="B26">
@@ -924,7 +924,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:41</t>
+          <t>02/03/2024 02:55:41</t>
         </is>
       </c>
       <c r="B27">
@@ -943,7 +943,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:51</t>
+          <t>02/03/2024 02:55:51</t>
         </is>
       </c>
       <c r="B28">
@@ -962,7 +962,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:01</t>
+          <t>02/03/2024 02:56:01</t>
         </is>
       </c>
       <c r="B29">
@@ -981,7 +981,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:11</t>
+          <t>02/03/2024 02:56:11</t>
         </is>
       </c>
       <c r="B30">
@@ -1000,7 +1000,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:21</t>
+          <t>02/03/2024 02:56:21</t>
         </is>
       </c>
       <c r="B31">
@@ -1019,7 +1019,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:31</t>
+          <t>02/03/2024 02:56:31</t>
         </is>
       </c>
       <c r="B32">
@@ -1038,7 +1038,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:41</t>
+          <t>02/03/2024 02:56:41</t>
         </is>
       </c>
       <c r="B33">
@@ -1057,7 +1057,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:51</t>
+          <t>02/03/2024 02:56:51</t>
         </is>
       </c>
       <c r="B34">
@@ -1076,7 +1076,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:01</t>
+          <t>02/03/2024 02:57:01</t>
         </is>
       </c>
       <c r="B35">
@@ -1095,7 +1095,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:11</t>
+          <t>02/03/2024 02:57:11</t>
         </is>
       </c>
       <c r="B36">
@@ -1114,7 +1114,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:21</t>
+          <t>02/03/2024 02:57:21</t>
         </is>
       </c>
       <c r="B37">
@@ -1133,7 +1133,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:31</t>
+          <t>02/03/2024 02:57:31</t>
         </is>
       </c>
       <c r="B38">
@@ -1152,7 +1152,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:41</t>
+          <t>02/03/2024 02:57:41</t>
         </is>
       </c>
       <c r="B39">
@@ -1171,7 +1171,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:51</t>
+          <t>02/03/2024 02:57:51</t>
         </is>
       </c>
       <c r="B40">
@@ -1190,7 +1190,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:01</t>
+          <t>02/03/2024 02:58:01</t>
         </is>
       </c>
       <c r="B41">
@@ -1209,7 +1209,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:11</t>
+          <t>02/03/2024 02:58:11</t>
         </is>
       </c>
       <c r="B42">
@@ -1228,7 +1228,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:21</t>
+          <t>02/03/2024 02:58:21</t>
         </is>
       </c>
       <c r="B43">
@@ -1247,7 +1247,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:31</t>
+          <t>02/03/2024 02:58:31</t>
         </is>
       </c>
       <c r="B44">
@@ -1266,7 +1266,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:41</t>
+          <t>02/03/2024 02:58:41</t>
         </is>
       </c>
       <c r="B45">
@@ -1285,7 +1285,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:51</t>
+          <t>02/03/2024 02:58:51</t>
         </is>
       </c>
       <c r="B46">
@@ -1304,7 +1304,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:01</t>
+          <t>02/03/2024 02:59:01</t>
         </is>
       </c>
       <c r="B47">
@@ -1323,7 +1323,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:11</t>
+          <t>02/03/2024 02:59:11</t>
         </is>
       </c>
       <c r="B48">
@@ -1342,7 +1342,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:21</t>
+          <t>02/03/2024 02:59:21</t>
         </is>
       </c>
       <c r="B49">
@@ -1361,7 +1361,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:31</t>
+          <t>02/03/2024 02:59:31</t>
         </is>
       </c>
       <c r="B50">
@@ -1380,7 +1380,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:41</t>
+          <t>02/03/2024 02:59:41</t>
         </is>
       </c>
       <c r="B51">
@@ -1399,7 +1399,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:51</t>
+          <t>02/03/2024 02:59:51</t>
         </is>
       </c>
       <c r="B52">
@@ -1418,7 +1418,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:01</t>
+          <t>02/03/2024 03:00:01</t>
         </is>
       </c>
       <c r="B53">
@@ -1437,7 +1437,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:11</t>
+          <t>02/03/2024 03:00:11</t>
         </is>
       </c>
       <c r="B54">
@@ -1456,7 +1456,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:21</t>
+          <t>02/03/2024 03:00:21</t>
         </is>
       </c>
       <c r="B55">
@@ -1475,7 +1475,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:31</t>
+          <t>02/03/2024 03:00:31</t>
         </is>
       </c>
       <c r="B56">
@@ -1494,7 +1494,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:41</t>
+          <t>02/03/2024 03:00:41</t>
         </is>
       </c>
       <c r="B57">
@@ -1513,7 +1513,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:51</t>
+          <t>02/03/2024 03:00:51</t>
         </is>
       </c>
       <c r="B58">
@@ -1532,7 +1532,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:01</t>
+          <t>02/03/2024 03:01:01</t>
         </is>
       </c>
       <c r="B59">
@@ -1551,7 +1551,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:11</t>
+          <t>02/03/2024 03:01:11</t>
         </is>
       </c>
       <c r="B60">
@@ -1570,7 +1570,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:21</t>
+          <t>02/03/2024 03:01:21</t>
         </is>
       </c>
       <c r="B61">
@@ -1589,7 +1589,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:31</t>
+          <t>02/03/2024 03:01:31</t>
         </is>
       </c>
       <c r="B62">
@@ -1608,7 +1608,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:41</t>
+          <t>02/03/2024 03:01:41</t>
         </is>
       </c>
       <c r="B63">
@@ -1627,7 +1627,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:51</t>
+          <t>02/03/2024 03:01:51</t>
         </is>
       </c>
       <c r="B64">
@@ -1646,7 +1646,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:01</t>
+          <t>02/03/2024 03:02:01</t>
         </is>
       </c>
       <c r="B65">
@@ -1665,7 +1665,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:11</t>
+          <t>02/03/2024 03:02:11</t>
         </is>
       </c>
       <c r="B66">
@@ -1684,7 +1684,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:21</t>
+          <t>02/03/2024 03:02:21</t>
         </is>
       </c>
       <c r="B67">
@@ -1703,7 +1703,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:31</t>
+          <t>02/03/2024 03:02:31</t>
         </is>
       </c>
       <c r="B68">
@@ -1722,7 +1722,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:41</t>
+          <t>02/03/2024 03:02:41</t>
         </is>
       </c>
       <c r="B69">
@@ -1741,7 +1741,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:51</t>
+          <t>02/03/2024 03:02:51</t>
         </is>
       </c>
       <c r="B70">
@@ -1760,7 +1760,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:01</t>
+          <t>02/03/2024 03:03:01</t>
         </is>
       </c>
       <c r="B71">
@@ -1779,7 +1779,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:11</t>
+          <t>02/03/2024 03:03:11</t>
         </is>
       </c>
       <c r="B72">
@@ -1798,7 +1798,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:21</t>
+          <t>02/03/2024 03:03:21</t>
         </is>
       </c>
       <c r="B73">
@@ -1817,7 +1817,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:31</t>
+          <t>02/03/2024 03:03:31</t>
         </is>
       </c>
       <c r="B74">
@@ -1836,7 +1836,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:41</t>
+          <t>02/03/2024 03:03:41</t>
         </is>
       </c>
       <c r="B75">
@@ -1855,7 +1855,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:51</t>
+          <t>02/03/2024 03:03:51</t>
         </is>
       </c>
       <c r="B76">
@@ -1874,7 +1874,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:01</t>
+          <t>02/03/2024 03:04:01</t>
         </is>
       </c>
       <c r="B77">
@@ -1893,7 +1893,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:11</t>
+          <t>02/03/2024 03:04:11</t>
         </is>
       </c>
       <c r="B78">
@@ -1912,7 +1912,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:21</t>
+          <t>02/03/2024 03:04:21</t>
         </is>
       </c>
       <c r="B79">
@@ -1931,7 +1931,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:31</t>
+          <t>02/03/2024 03:04:31</t>
         </is>
       </c>
       <c r="B80">
@@ -1950,7 +1950,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:41</t>
+          <t>02/03/2024 03:04:41</t>
         </is>
       </c>
       <c r="B81">
@@ -2013,7 +2013,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:35</t>
+          <t>02/03/2024 02:51:35</t>
         </is>
       </c>
       <c r="B2">
@@ -2032,7 +2032,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:45</t>
+          <t>02/03/2024 02:51:45</t>
         </is>
       </c>
       <c r="B3">
@@ -2051,7 +2051,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:55</t>
+          <t>02/03/2024 02:51:55</t>
         </is>
       </c>
       <c r="B4">
@@ -2070,7 +2070,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:05</t>
+          <t>02/03/2024 02:52:05</t>
         </is>
       </c>
       <c r="B5">
@@ -2089,7 +2089,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:15</t>
+          <t>02/03/2024 02:52:15</t>
         </is>
       </c>
       <c r="B6">
@@ -2108,7 +2108,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:25</t>
+          <t>02/03/2024 02:52:25</t>
         </is>
       </c>
       <c r="B7">
@@ -2127,7 +2127,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:35</t>
+          <t>02/03/2024 02:52:35</t>
         </is>
       </c>
       <c r="B8">
@@ -2146,7 +2146,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:45</t>
+          <t>02/03/2024 02:52:45</t>
         </is>
       </c>
       <c r="B9">
@@ -2165,7 +2165,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:55</t>
+          <t>02/03/2024 02:52:55</t>
         </is>
       </c>
       <c r="B10">
@@ -2184,7 +2184,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:05</t>
+          <t>02/03/2024 02:53:05</t>
         </is>
       </c>
       <c r="B11">
@@ -2203,7 +2203,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:15</t>
+          <t>02/03/2024 02:53:15</t>
         </is>
       </c>
       <c r="B12">
@@ -2222,7 +2222,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:25</t>
+          <t>02/03/2024 02:53:25</t>
         </is>
       </c>
       <c r="B13">
@@ -2241,7 +2241,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:35</t>
+          <t>02/03/2024 02:53:35</t>
         </is>
       </c>
       <c r="B14">
@@ -2260,7 +2260,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:45</t>
+          <t>02/03/2024 02:53:45</t>
         </is>
       </c>
       <c r="B15">
@@ -2279,7 +2279,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:55</t>
+          <t>02/03/2024 02:53:55</t>
         </is>
       </c>
       <c r="B16">
@@ -2298,7 +2298,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:05</t>
+          <t>02/03/2024 02:54:05</t>
         </is>
       </c>
       <c r="B17">
@@ -2317,7 +2317,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:15</t>
+          <t>02/03/2024 02:54:15</t>
         </is>
       </c>
       <c r="B18">
@@ -2336,7 +2336,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:25</t>
+          <t>02/03/2024 02:54:25</t>
         </is>
       </c>
       <c r="B19">
@@ -2355,7 +2355,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:35</t>
+          <t>02/03/2024 02:54:35</t>
         </is>
       </c>
       <c r="B20">
@@ -2374,7 +2374,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:45</t>
+          <t>02/03/2024 02:54:45</t>
         </is>
       </c>
       <c r="B21">
@@ -2393,7 +2393,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:55</t>
+          <t>02/03/2024 02:54:55</t>
         </is>
       </c>
       <c r="B22">
@@ -2412,7 +2412,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:05</t>
+          <t>02/03/2024 02:55:05</t>
         </is>
       </c>
       <c r="B23">
@@ -2431,7 +2431,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:15</t>
+          <t>02/03/2024 02:55:15</t>
         </is>
       </c>
       <c r="B24">
@@ -2450,7 +2450,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:25</t>
+          <t>02/03/2024 02:55:25</t>
         </is>
       </c>
       <c r="B25">
@@ -2469,7 +2469,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:35</t>
+          <t>02/03/2024 02:55:35</t>
         </is>
       </c>
       <c r="B26">
@@ -2488,7 +2488,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:45</t>
+          <t>02/03/2024 02:55:45</t>
         </is>
       </c>
       <c r="B27">
@@ -2507,7 +2507,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:55</t>
+          <t>02/03/2024 02:55:55</t>
         </is>
       </c>
       <c r="B28">
@@ -2526,7 +2526,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:05</t>
+          <t>02/03/2024 02:56:05</t>
         </is>
       </c>
       <c r="B29">
@@ -2545,7 +2545,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:15</t>
+          <t>02/03/2024 02:56:15</t>
         </is>
       </c>
       <c r="B30">
@@ -2564,7 +2564,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:25</t>
+          <t>02/03/2024 02:56:25</t>
         </is>
       </c>
       <c r="B31">
@@ -2583,7 +2583,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:35</t>
+          <t>02/03/2024 02:56:35</t>
         </is>
       </c>
       <c r="B32">
@@ -2602,7 +2602,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:45</t>
+          <t>02/03/2024 02:56:45</t>
         </is>
       </c>
       <c r="B33">
@@ -2621,7 +2621,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:55</t>
+          <t>02/03/2024 02:56:55</t>
         </is>
       </c>
       <c r="B34">
@@ -2640,7 +2640,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:05</t>
+          <t>02/03/2024 02:57:05</t>
         </is>
       </c>
       <c r="B35">
@@ -2659,7 +2659,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:15</t>
+          <t>02/03/2024 02:57:15</t>
         </is>
       </c>
       <c r="B36">
@@ -2678,7 +2678,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:25</t>
+          <t>02/03/2024 02:57:25</t>
         </is>
       </c>
       <c r="B37">
@@ -2697,7 +2697,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:35</t>
+          <t>02/03/2024 02:57:35</t>
         </is>
       </c>
       <c r="B38">
@@ -2716,7 +2716,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:45</t>
+          <t>02/03/2024 02:57:45</t>
         </is>
       </c>
       <c r="B39">
@@ -2735,7 +2735,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:55</t>
+          <t>02/03/2024 02:57:55</t>
         </is>
       </c>
       <c r="B40">
@@ -2754,7 +2754,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:05</t>
+          <t>02/03/2024 02:58:05</t>
         </is>
       </c>
       <c r="B41">
@@ -2773,7 +2773,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:15</t>
+          <t>02/03/2024 02:58:15</t>
         </is>
       </c>
       <c r="B42">
@@ -2792,7 +2792,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:25</t>
+          <t>02/03/2024 02:58:25</t>
         </is>
       </c>
       <c r="B43">
@@ -2811,7 +2811,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:35</t>
+          <t>02/03/2024 02:58:35</t>
         </is>
       </c>
       <c r="B44">
@@ -2830,7 +2830,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:45</t>
+          <t>02/03/2024 02:58:45</t>
         </is>
       </c>
       <c r="B45">
@@ -2849,7 +2849,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:55</t>
+          <t>02/03/2024 02:58:55</t>
         </is>
       </c>
       <c r="B46">
@@ -2868,7 +2868,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:05</t>
+          <t>02/03/2024 02:59:05</t>
         </is>
       </c>
       <c r="B47">
@@ -2887,7 +2887,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:15</t>
+          <t>02/03/2024 02:59:15</t>
         </is>
       </c>
       <c r="B48">
@@ -2906,7 +2906,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:25</t>
+          <t>02/03/2024 02:59:25</t>
         </is>
       </c>
       <c r="B49">
@@ -2925,7 +2925,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:35</t>
+          <t>02/03/2024 02:59:35</t>
         </is>
       </c>
       <c r="B50">
@@ -2944,7 +2944,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:45</t>
+          <t>02/03/2024 02:59:45</t>
         </is>
       </c>
       <c r="B51">
@@ -2963,7 +2963,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:55</t>
+          <t>02/03/2024 02:59:55</t>
         </is>
       </c>
       <c r="B52">
@@ -2982,7 +2982,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:05</t>
+          <t>02/03/2024 03:00:05</t>
         </is>
       </c>
       <c r="B53">
@@ -3001,7 +3001,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:15</t>
+          <t>02/03/2024 03:00:15</t>
         </is>
       </c>
       <c r="B54">
@@ -3020,7 +3020,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:25</t>
+          <t>02/03/2024 03:00:25</t>
         </is>
       </c>
       <c r="B55">
@@ -3039,7 +3039,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:35</t>
+          <t>02/03/2024 03:00:35</t>
         </is>
       </c>
       <c r="B56">
@@ -3058,7 +3058,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:45</t>
+          <t>02/03/2024 03:00:45</t>
         </is>
       </c>
       <c r="B57">
@@ -3077,7 +3077,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:55</t>
+          <t>02/03/2024 03:00:55</t>
         </is>
       </c>
       <c r="B58">
@@ -3096,7 +3096,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:05</t>
+          <t>02/03/2024 03:01:05</t>
         </is>
       </c>
       <c r="B59">
@@ -3115,7 +3115,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:15</t>
+          <t>02/03/2024 03:01:15</t>
         </is>
       </c>
       <c r="B60">
@@ -3134,7 +3134,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:25</t>
+          <t>02/03/2024 03:01:25</t>
         </is>
       </c>
       <c r="B61">
@@ -3153,7 +3153,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:35</t>
+          <t>02/03/2024 03:01:35</t>
         </is>
       </c>
       <c r="B62">
@@ -3172,7 +3172,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:45</t>
+          <t>02/03/2024 03:01:45</t>
         </is>
       </c>
       <c r="B63">
@@ -3191,7 +3191,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:55</t>
+          <t>02/03/2024 03:01:55</t>
         </is>
       </c>
       <c r="B64">
@@ -3210,7 +3210,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:05</t>
+          <t>02/03/2024 03:02:05</t>
         </is>
       </c>
       <c r="B65">
@@ -3229,7 +3229,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:15</t>
+          <t>02/03/2024 03:02:15</t>
         </is>
       </c>
       <c r="B66">
@@ -3248,7 +3248,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:25</t>
+          <t>02/03/2024 03:02:25</t>
         </is>
       </c>
       <c r="B67">
@@ -3267,7 +3267,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:35</t>
+          <t>02/03/2024 03:02:35</t>
         </is>
       </c>
       <c r="B68">
@@ -3286,7 +3286,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:45</t>
+          <t>02/03/2024 03:02:45</t>
         </is>
       </c>
       <c r="B69">
@@ -3305,7 +3305,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:55</t>
+          <t>02/03/2024 03:02:55</t>
         </is>
       </c>
       <c r="B70">
@@ -3324,7 +3324,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:05</t>
+          <t>02/03/2024 03:03:05</t>
         </is>
       </c>
       <c r="B71">
@@ -3343,7 +3343,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:15</t>
+          <t>02/03/2024 03:03:15</t>
         </is>
       </c>
       <c r="B72">
@@ -3362,7 +3362,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:25</t>
+          <t>02/03/2024 03:03:25</t>
         </is>
       </c>
       <c r="B73">
@@ -3381,7 +3381,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:35</t>
+          <t>02/03/2024 03:03:35</t>
         </is>
       </c>
       <c r="B74">
@@ -3400,7 +3400,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:45</t>
+          <t>02/03/2024 03:03:45</t>
         </is>
       </c>
       <c r="B75">
@@ -3419,7 +3419,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:55</t>
+          <t>02/03/2024 03:03:55</t>
         </is>
       </c>
       <c r="B76">
@@ -3438,7 +3438,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:05</t>
+          <t>02/03/2024 03:04:05</t>
         </is>
       </c>
       <c r="B77">
@@ -3457,7 +3457,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:15</t>
+          <t>02/03/2024 03:04:15</t>
         </is>
       </c>
       <c r="B78">
@@ -3476,7 +3476,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:25</t>
+          <t>02/03/2024 03:04:25</t>
         </is>
       </c>
       <c r="B79">
@@ -3495,7 +3495,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:35</t>
+          <t>02/03/2024 03:04:35</t>
         </is>
       </c>
       <c r="B80">
@@ -3514,7 +3514,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:45</t>
+          <t>02/03/2024 03:04:45</t>
         </is>
       </c>
       <c r="B81">
@@ -3577,7 +3577,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:37</t>
+          <t>02/03/2024 02:51:37</t>
         </is>
       </c>
       <c r="B2">
@@ -3596,7 +3596,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:47</t>
+          <t>02/03/2024 02:51:47</t>
         </is>
       </c>
       <c r="B3">
@@ -3615,7 +3615,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:57</t>
+          <t>02/03/2024 02:51:57</t>
         </is>
       </c>
       <c r="B4">
@@ -3634,7 +3634,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:07</t>
+          <t>02/03/2024 02:52:07</t>
         </is>
       </c>
       <c r="B5">
@@ -3653,7 +3653,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:17</t>
+          <t>02/03/2024 02:52:17</t>
         </is>
       </c>
       <c r="B6">
@@ -3672,7 +3672,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:27</t>
+          <t>02/03/2024 02:52:27</t>
         </is>
       </c>
       <c r="B7">
@@ -3691,7 +3691,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:37</t>
+          <t>02/03/2024 02:52:37</t>
         </is>
       </c>
       <c r="B8">
@@ -3710,7 +3710,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:47</t>
+          <t>02/03/2024 02:52:47</t>
         </is>
       </c>
       <c r="B9">
@@ -3729,7 +3729,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:57</t>
+          <t>02/03/2024 02:52:57</t>
         </is>
       </c>
       <c r="B10">
@@ -3748,7 +3748,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:07</t>
+          <t>02/03/2024 02:53:07</t>
         </is>
       </c>
       <c r="B11">
@@ -3767,7 +3767,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:17</t>
+          <t>02/03/2024 02:53:17</t>
         </is>
       </c>
       <c r="B12">
@@ -3786,7 +3786,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:27</t>
+          <t>02/03/2024 02:53:27</t>
         </is>
       </c>
       <c r="B13">
@@ -3805,7 +3805,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:37</t>
+          <t>02/03/2024 02:53:37</t>
         </is>
       </c>
       <c r="B14">
@@ -3824,7 +3824,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:47</t>
+          <t>02/03/2024 02:53:47</t>
         </is>
       </c>
       <c r="B15">
@@ -3843,7 +3843,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:57</t>
+          <t>02/03/2024 02:53:57</t>
         </is>
       </c>
       <c r="B16">
@@ -3862,7 +3862,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:07</t>
+          <t>02/03/2024 02:54:07</t>
         </is>
       </c>
       <c r="B17">
@@ -3881,7 +3881,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:17</t>
+          <t>02/03/2024 02:54:17</t>
         </is>
       </c>
       <c r="B18">
@@ -3900,7 +3900,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:27</t>
+          <t>02/03/2024 02:54:27</t>
         </is>
       </c>
       <c r="B19">
@@ -3919,7 +3919,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:37</t>
+          <t>02/03/2024 02:54:37</t>
         </is>
       </c>
       <c r="B20">
@@ -3938,7 +3938,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:47</t>
+          <t>02/03/2024 02:54:47</t>
         </is>
       </c>
       <c r="B21">
@@ -3957,7 +3957,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:57</t>
+          <t>02/03/2024 02:54:57</t>
         </is>
       </c>
       <c r="B22">
@@ -3976,7 +3976,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:07</t>
+          <t>02/03/2024 02:55:07</t>
         </is>
       </c>
       <c r="B23">
@@ -3995,7 +3995,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:17</t>
+          <t>02/03/2024 02:55:17</t>
         </is>
       </c>
       <c r="B24">
@@ -4014,7 +4014,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:27</t>
+          <t>02/03/2024 02:55:27</t>
         </is>
       </c>
       <c r="B25">
@@ -4033,7 +4033,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:37</t>
+          <t>02/03/2024 02:55:37</t>
         </is>
       </c>
       <c r="B26">
@@ -4052,7 +4052,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:47</t>
+          <t>02/03/2024 02:55:47</t>
         </is>
       </c>
       <c r="B27">
@@ -4071,7 +4071,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:57</t>
+          <t>02/03/2024 02:55:57</t>
         </is>
       </c>
       <c r="B28">
@@ -4090,7 +4090,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:07</t>
+          <t>02/03/2024 02:56:07</t>
         </is>
       </c>
       <c r="B29">
@@ -4109,7 +4109,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:17</t>
+          <t>02/03/2024 02:56:17</t>
         </is>
       </c>
       <c r="B30">
@@ -4128,7 +4128,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:27</t>
+          <t>02/03/2024 02:56:27</t>
         </is>
       </c>
       <c r="B31">
@@ -4147,7 +4147,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:37</t>
+          <t>02/03/2024 02:56:37</t>
         </is>
       </c>
       <c r="B32">
@@ -4166,7 +4166,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:47</t>
+          <t>02/03/2024 02:56:47</t>
         </is>
       </c>
       <c r="B33">
@@ -4185,7 +4185,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:57</t>
+          <t>02/03/2024 02:56:57</t>
         </is>
       </c>
       <c r="B34">
@@ -4204,7 +4204,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:07</t>
+          <t>02/03/2024 02:57:07</t>
         </is>
       </c>
       <c r="B35">
@@ -4223,7 +4223,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:17</t>
+          <t>02/03/2024 02:57:17</t>
         </is>
       </c>
       <c r="B36">
@@ -4242,7 +4242,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:27</t>
+          <t>02/03/2024 02:57:27</t>
         </is>
       </c>
       <c r="B37">
@@ -4261,7 +4261,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:37</t>
+          <t>02/03/2024 02:57:37</t>
         </is>
       </c>
       <c r="B38">
@@ -4280,7 +4280,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:47</t>
+          <t>02/03/2024 02:57:47</t>
         </is>
       </c>
       <c r="B39">
@@ -4299,7 +4299,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:57</t>
+          <t>02/03/2024 02:57:57</t>
         </is>
       </c>
       <c r="B40">
@@ -4318,7 +4318,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:07</t>
+          <t>02/03/2024 02:58:07</t>
         </is>
       </c>
       <c r="B41">
@@ -4337,7 +4337,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:17</t>
+          <t>02/03/2024 02:58:17</t>
         </is>
       </c>
       <c r="B42">
@@ -4356,7 +4356,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:27</t>
+          <t>02/03/2024 02:58:27</t>
         </is>
       </c>
       <c r="B43">
@@ -4375,7 +4375,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:37</t>
+          <t>02/03/2024 02:58:37</t>
         </is>
       </c>
       <c r="B44">
@@ -4394,7 +4394,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:47</t>
+          <t>02/03/2024 02:58:47</t>
         </is>
       </c>
       <c r="B45">
@@ -4413,7 +4413,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:57</t>
+          <t>02/03/2024 02:58:57</t>
         </is>
       </c>
       <c r="B46">
@@ -4432,7 +4432,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:07</t>
+          <t>02/03/2024 02:59:07</t>
         </is>
       </c>
       <c r="B47">
@@ -4451,7 +4451,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:17</t>
+          <t>02/03/2024 02:59:17</t>
         </is>
       </c>
       <c r="B48">
@@ -4470,7 +4470,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:27</t>
+          <t>02/03/2024 02:59:27</t>
         </is>
       </c>
       <c r="B49">
@@ -4489,7 +4489,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:37</t>
+          <t>02/03/2024 02:59:37</t>
         </is>
       </c>
       <c r="B50">
@@ -4508,7 +4508,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:47</t>
+          <t>02/03/2024 02:59:47</t>
         </is>
       </c>
       <c r="B51">
@@ -4527,7 +4527,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:57</t>
+          <t>02/03/2024 02:59:57</t>
         </is>
       </c>
       <c r="B52">
@@ -4546,7 +4546,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:07</t>
+          <t>02/03/2024 03:00:07</t>
         </is>
       </c>
       <c r="B53">
@@ -4565,7 +4565,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:17</t>
+          <t>02/03/2024 03:00:17</t>
         </is>
       </c>
       <c r="B54">
@@ -4584,7 +4584,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:27</t>
+          <t>02/03/2024 03:00:27</t>
         </is>
       </c>
       <c r="B55">
@@ -4603,7 +4603,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:37</t>
+          <t>02/03/2024 03:00:37</t>
         </is>
       </c>
       <c r="B56">
@@ -4622,7 +4622,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:47</t>
+          <t>02/03/2024 03:00:47</t>
         </is>
       </c>
       <c r="B57">
@@ -4641,7 +4641,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:57</t>
+          <t>02/03/2024 03:00:57</t>
         </is>
       </c>
       <c r="B58">
@@ -4660,7 +4660,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:07</t>
+          <t>02/03/2024 03:01:07</t>
         </is>
       </c>
       <c r="B59">
@@ -4679,7 +4679,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:17</t>
+          <t>02/03/2024 03:01:17</t>
         </is>
       </c>
       <c r="B60">
@@ -4698,7 +4698,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:27</t>
+          <t>02/03/2024 03:01:27</t>
         </is>
       </c>
       <c r="B61">
@@ -4717,7 +4717,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:37</t>
+          <t>02/03/2024 03:01:37</t>
         </is>
       </c>
       <c r="B62">
@@ -4736,7 +4736,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:47</t>
+          <t>02/03/2024 03:01:47</t>
         </is>
       </c>
       <c r="B63">
@@ -4755,7 +4755,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:57</t>
+          <t>02/03/2024 03:01:57</t>
         </is>
       </c>
       <c r="B64">
@@ -4774,7 +4774,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:07</t>
+          <t>02/03/2024 03:02:07</t>
         </is>
       </c>
       <c r="B65">
@@ -4793,7 +4793,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:17</t>
+          <t>02/03/2024 03:02:17</t>
         </is>
       </c>
       <c r="B66">
@@ -4812,7 +4812,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:27</t>
+          <t>02/03/2024 03:02:27</t>
         </is>
       </c>
       <c r="B67">
@@ -4831,7 +4831,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:37</t>
+          <t>02/03/2024 03:02:37</t>
         </is>
       </c>
       <c r="B68">
@@ -4850,7 +4850,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:47</t>
+          <t>02/03/2024 03:02:47</t>
         </is>
       </c>
       <c r="B69">
@@ -4869,7 +4869,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:57</t>
+          <t>02/03/2024 03:02:57</t>
         </is>
       </c>
       <c r="B70">
@@ -4888,7 +4888,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:07</t>
+          <t>02/03/2024 03:03:07</t>
         </is>
       </c>
       <c r="B71">
@@ -4907,7 +4907,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:17</t>
+          <t>02/03/2024 03:03:17</t>
         </is>
       </c>
       <c r="B72">
@@ -4926,7 +4926,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:27</t>
+          <t>02/03/2024 03:03:27</t>
         </is>
       </c>
       <c r="B73">
@@ -4945,7 +4945,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:37</t>
+          <t>02/03/2024 03:03:37</t>
         </is>
       </c>
       <c r="B74">
@@ -4964,7 +4964,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:47</t>
+          <t>02/03/2024 03:03:47</t>
         </is>
       </c>
       <c r="B75">
@@ -4983,7 +4983,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:57</t>
+          <t>02/03/2024 03:03:57</t>
         </is>
       </c>
       <c r="B76">
@@ -5002,7 +5002,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:07</t>
+          <t>02/03/2024 03:04:07</t>
         </is>
       </c>
       <c r="B77">
@@ -5021,7 +5021,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:17</t>
+          <t>02/03/2024 03:04:17</t>
         </is>
       </c>
       <c r="B78">
@@ -5040,7 +5040,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:27</t>
+          <t>02/03/2024 03:04:27</t>
         </is>
       </c>
       <c r="B79">
@@ -5059,7 +5059,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:37</t>
+          <t>02/03/2024 03:04:37</t>
         </is>
       </c>
       <c r="B80">
@@ -5078,7 +5078,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:47</t>
+          <t>02/03/2024 03:04:47</t>
         </is>
       </c>
       <c r="B81">
@@ -5141,7 +5141,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:39</t>
+          <t>02/03/2024 02:51:39</t>
         </is>
       </c>
       <c r="B2">
@@ -5160,7 +5160,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:49</t>
+          <t>02/03/2024 02:51:49</t>
         </is>
       </c>
       <c r="B3">
@@ -5179,7 +5179,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/02/2024 02:51:59</t>
+          <t>02/03/2024 02:51:59</t>
         </is>
       </c>
       <c r="B4">
@@ -5198,7 +5198,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:09</t>
+          <t>02/03/2024 02:52:09</t>
         </is>
       </c>
       <c r="B5">
@@ -5217,7 +5217,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:19</t>
+          <t>02/03/2024 02:52:19</t>
         </is>
       </c>
       <c r="B6">
@@ -5236,7 +5236,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:29</t>
+          <t>02/03/2024 02:52:29</t>
         </is>
       </c>
       <c r="B7">
@@ -5255,7 +5255,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:39</t>
+          <t>02/03/2024 02:52:39</t>
         </is>
       </c>
       <c r="B8">
@@ -5274,7 +5274,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:49</t>
+          <t>02/03/2024 02:52:49</t>
         </is>
       </c>
       <c r="B9">
@@ -5293,7 +5293,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03/02/2024 02:52:59</t>
+          <t>02/03/2024 02:52:59</t>
         </is>
       </c>
       <c r="B10">
@@ -5312,7 +5312,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:09</t>
+          <t>02/03/2024 02:53:09</t>
         </is>
       </c>
       <c r="B11">
@@ -5331,7 +5331,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:19</t>
+          <t>02/03/2024 02:53:19</t>
         </is>
       </c>
       <c r="B12">
@@ -5350,7 +5350,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:29</t>
+          <t>02/03/2024 02:53:29</t>
         </is>
       </c>
       <c r="B13">
@@ -5369,7 +5369,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:39</t>
+          <t>02/03/2024 02:53:39</t>
         </is>
       </c>
       <c r="B14">
@@ -5388,7 +5388,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:49</t>
+          <t>02/03/2024 02:53:49</t>
         </is>
       </c>
       <c r="B15">
@@ -5407,7 +5407,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03/02/2024 02:53:59</t>
+          <t>02/03/2024 02:53:59</t>
         </is>
       </c>
       <c r="B16">
@@ -5426,7 +5426,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:09</t>
+          <t>02/03/2024 02:54:09</t>
         </is>
       </c>
       <c r="B17">
@@ -5445,7 +5445,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:19</t>
+          <t>02/03/2024 02:54:19</t>
         </is>
       </c>
       <c r="B18">
@@ -5464,7 +5464,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:29</t>
+          <t>02/03/2024 02:54:29</t>
         </is>
       </c>
       <c r="B19">
@@ -5483,7 +5483,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:39</t>
+          <t>02/03/2024 02:54:39</t>
         </is>
       </c>
       <c r="B20">
@@ -5502,7 +5502,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:49</t>
+          <t>02/03/2024 02:54:49</t>
         </is>
       </c>
       <c r="B21">
@@ -5521,7 +5521,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03/02/2024 02:54:59</t>
+          <t>02/03/2024 02:54:59</t>
         </is>
       </c>
       <c r="B22">
@@ -5540,7 +5540,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:09</t>
+          <t>02/03/2024 02:55:09</t>
         </is>
       </c>
       <c r="B23">
@@ -5559,7 +5559,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:19</t>
+          <t>02/03/2024 02:55:19</t>
         </is>
       </c>
       <c r="B24">
@@ -5578,7 +5578,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:29</t>
+          <t>02/03/2024 02:55:29</t>
         </is>
       </c>
       <c r="B25">
@@ -5597,7 +5597,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:39</t>
+          <t>02/03/2024 02:55:39</t>
         </is>
       </c>
       <c r="B26">
@@ -5616,7 +5616,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:49</t>
+          <t>02/03/2024 02:55:49</t>
         </is>
       </c>
       <c r="B27">
@@ -5635,7 +5635,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/02/2024 02:55:59</t>
+          <t>02/03/2024 02:55:59</t>
         </is>
       </c>
       <c r="B28">
@@ -5654,7 +5654,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:09</t>
+          <t>02/03/2024 02:56:09</t>
         </is>
       </c>
       <c r="B29">
@@ -5673,7 +5673,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:19</t>
+          <t>02/03/2024 02:56:19</t>
         </is>
       </c>
       <c r="B30">
@@ -5692,7 +5692,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:29</t>
+          <t>02/03/2024 02:56:29</t>
         </is>
       </c>
       <c r="B31">
@@ -5711,7 +5711,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:39</t>
+          <t>02/03/2024 02:56:39</t>
         </is>
       </c>
       <c r="B32">
@@ -5730,7 +5730,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:49</t>
+          <t>02/03/2024 02:56:49</t>
         </is>
       </c>
       <c r="B33">
@@ -5749,7 +5749,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>03/02/2024 02:56:59</t>
+          <t>02/03/2024 02:56:59</t>
         </is>
       </c>
       <c r="B34">
@@ -5768,7 +5768,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:09</t>
+          <t>02/03/2024 02:57:09</t>
         </is>
       </c>
       <c r="B35">
@@ -5787,7 +5787,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:19</t>
+          <t>02/03/2024 02:57:19</t>
         </is>
       </c>
       <c r="B36">
@@ -5806,7 +5806,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:29</t>
+          <t>02/03/2024 02:57:29</t>
         </is>
       </c>
       <c r="B37">
@@ -5825,7 +5825,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:39</t>
+          <t>02/03/2024 02:57:39</t>
         </is>
       </c>
       <c r="B38">
@@ -5844,7 +5844,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>03/02/2024 02:57:59</t>
+          <t>02/03/2024 02:57:59</t>
         </is>
       </c>
       <c r="B39">
@@ -5863,7 +5863,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:09</t>
+          <t>02/03/2024 02:58:09</t>
         </is>
       </c>
       <c r="B40">
@@ -5882,7 +5882,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:19</t>
+          <t>02/03/2024 02:58:19</t>
         </is>
       </c>
       <c r="B41">
@@ -5901,7 +5901,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:29</t>
+          <t>02/03/2024 02:58:29</t>
         </is>
       </c>
       <c r="B42">
@@ -5920,7 +5920,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:39</t>
+          <t>02/03/2024 02:58:39</t>
         </is>
       </c>
       <c r="B43">
@@ -5939,7 +5939,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:49</t>
+          <t>02/03/2024 02:58:49</t>
         </is>
       </c>
       <c r="B44">
@@ -5958,7 +5958,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>03/02/2024 02:58:59</t>
+          <t>02/03/2024 02:58:59</t>
         </is>
       </c>
       <c r="B45">
@@ -5977,7 +5977,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:09</t>
+          <t>02/03/2024 02:59:09</t>
         </is>
       </c>
       <c r="B46">
@@ -5996,7 +5996,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:19</t>
+          <t>02/03/2024 02:59:19</t>
         </is>
       </c>
       <c r="B47">
@@ -6015,7 +6015,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:29</t>
+          <t>02/03/2024 02:59:29</t>
         </is>
       </c>
       <c r="B48">
@@ -6034,7 +6034,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:39</t>
+          <t>02/03/2024 02:59:39</t>
         </is>
       </c>
       <c r="B49">
@@ -6053,7 +6053,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:49</t>
+          <t>02/03/2024 02:59:49</t>
         </is>
       </c>
       <c r="B50">
@@ -6072,7 +6072,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>03/02/2024 02:59:59</t>
+          <t>02/03/2024 02:59:59</t>
         </is>
       </c>
       <c r="B51">
@@ -6091,7 +6091,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:09</t>
+          <t>02/03/2024 03:00:09</t>
         </is>
       </c>
       <c r="B52">
@@ -6110,7 +6110,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:19</t>
+          <t>02/03/2024 03:00:19</t>
         </is>
       </c>
       <c r="B53">
@@ -6129,7 +6129,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:29</t>
+          <t>02/03/2024 03:00:29</t>
         </is>
       </c>
       <c r="B54">
@@ -6148,7 +6148,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:39</t>
+          <t>02/03/2024 03:00:39</t>
         </is>
       </c>
       <c r="B55">
@@ -6167,7 +6167,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:49</t>
+          <t>02/03/2024 03:00:49</t>
         </is>
       </c>
       <c r="B56">
@@ -6186,7 +6186,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>03/02/2024 03:00:59</t>
+          <t>02/03/2024 03:00:59</t>
         </is>
       </c>
       <c r="B57">
@@ -6205,7 +6205,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:09</t>
+          <t>02/03/2024 03:01:09</t>
         </is>
       </c>
       <c r="B58">
@@ -6224,7 +6224,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:19</t>
+          <t>02/03/2024 03:01:19</t>
         </is>
       </c>
       <c r="B59">
@@ -6243,7 +6243,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:29</t>
+          <t>02/03/2024 03:01:29</t>
         </is>
       </c>
       <c r="B60">
@@ -6262,7 +6262,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:39</t>
+          <t>02/03/2024 03:01:39</t>
         </is>
       </c>
       <c r="B61">
@@ -6281,7 +6281,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:49</t>
+          <t>02/03/2024 03:01:49</t>
         </is>
       </c>
       <c r="B62">
@@ -6300,7 +6300,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>03/02/2024 03:01:59</t>
+          <t>02/03/2024 03:01:59</t>
         </is>
       </c>
       <c r="B63">
@@ -6319,7 +6319,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:09</t>
+          <t>02/03/2024 03:02:09</t>
         </is>
       </c>
       <c r="B64">
@@ -6338,7 +6338,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:19</t>
+          <t>02/03/2024 03:02:19</t>
         </is>
       </c>
       <c r="B65">
@@ -6357,7 +6357,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:29</t>
+          <t>02/03/2024 03:02:29</t>
         </is>
       </c>
       <c r="B66">
@@ -6376,7 +6376,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:39</t>
+          <t>02/03/2024 03:02:39</t>
         </is>
       </c>
       <c r="B67">
@@ -6395,7 +6395,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:49</t>
+          <t>02/03/2024 03:02:49</t>
         </is>
       </c>
       <c r="B68">
@@ -6414,7 +6414,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>03/02/2024 03:02:59</t>
+          <t>02/03/2024 03:02:59</t>
         </is>
       </c>
       <c r="B69">
@@ -6433,7 +6433,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:09</t>
+          <t>02/03/2024 03:03:09</t>
         </is>
       </c>
       <c r="B70">
@@ -6452,7 +6452,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:19</t>
+          <t>02/03/2024 03:03:19</t>
         </is>
       </c>
       <c r="B71">
@@ -6471,7 +6471,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:29</t>
+          <t>02/03/2024 03:03:29</t>
         </is>
       </c>
       <c r="B72">
@@ -6490,7 +6490,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:39</t>
+          <t>02/03/2024 03:03:39</t>
         </is>
       </c>
       <c r="B73">
@@ -6509,7 +6509,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:49</t>
+          <t>02/03/2024 03:03:49</t>
         </is>
       </c>
       <c r="B74">
@@ -6528,7 +6528,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>03/02/2024 03:03:59</t>
+          <t>02/03/2024 03:03:59</t>
         </is>
       </c>
       <c r="B75">
@@ -6547,7 +6547,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:09</t>
+          <t>02/03/2024 03:04:09</t>
         </is>
       </c>
       <c r="B76">
@@ -6566,7 +6566,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:19</t>
+          <t>02/03/2024 03:04:19</t>
         </is>
       </c>
       <c r="B77">
@@ -6585,7 +6585,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:29</t>
+          <t>02/03/2024 03:04:29</t>
         </is>
       </c>
       <c r="B78">
@@ -6604,7 +6604,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:39</t>
+          <t>02/03/2024 03:04:39</t>
         </is>
       </c>
       <c r="B79">
@@ -6623,7 +6623,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>03/02/2024 03:04:49</t>
+          <t>02/03/2024 03:04:49</t>
         </is>
       </c>
       <c r="B80">

</xml_diff>